<commit_message>
feat: add kuota field to matkul and update related features
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t xml:space="preserve">nama</t>
   </si>
   <si>
-    <t xml:space="preserve">kode</t>
+    <t xml:space="preserve">kuota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kode_matkul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">semester</t>
   </si>
   <si>
     <t xml:space="preserve">coba</t>
@@ -43,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -234,10 +241,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,13 +256,25 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>